<commit_message>
Agregado de estado de tarea
</commit_message>
<xml_diff>
--- a/Lista de tareas individuales/Lista_Tareas_Revision_1_-_David_Barcenas_Duran.xlsx
+++ b/Lista de tareas individuales/Lista_Tareas_Revision_1_-_David_Barcenas_Duran.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bestr\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bestr\Desktop\Repositorios\ItaliaPizza-doc\Lista de tareas individuales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C15C96-1D31-4C10-A28C-B0FD6C5EB5B1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E50546B-3126-4086-ADF0-1260C1BD9DB1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="79">
   <si>
     <t>Columna</t>
   </si>
@@ -219,9 +219,6 @@
     <t>DBD, JAGL, GSC</t>
   </si>
   <si>
-    <t>Por iniciar</t>
-  </si>
-  <si>
     <t>Editar pedido</t>
   </si>
   <si>
@@ -274,6 +271,12 @@
   </si>
   <si>
     <t>Generar reporte de venta</t>
+  </si>
+  <si>
+    <t>Terminado</t>
+  </si>
+  <si>
+    <t>No aplica</t>
   </si>
 </sst>
 </file>
@@ -784,10 +787,10 @@
   <dimension ref="B1:BA56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="W6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AZ6" sqref="AZ6:AZ56"/>
+      <selection pane="bottomRight" activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1088,7 +1091,7 @@
         <v>58</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G6" s="5">
         <v>5</v>
@@ -1200,7 +1203,7 @@
         <v>58</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G7" s="5">
         <v>3</v>
@@ -1312,7 +1315,7 @@
         <v>58</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G8" s="5">
         <v>4</v>
@@ -1419,7 +1422,7 @@
         <v>47</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>43</v>
@@ -1428,7 +1431,7 @@
         <v>54</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G9" s="5">
         <v>2</v>
@@ -1540,7 +1543,7 @@
         <v>54</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G10" s="5">
         <v>1</v>
@@ -1652,7 +1655,7 @@
         <v>54</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G11" s="5">
         <v>2</v>
@@ -1764,7 +1767,7 @@
         <v>54</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G12" s="5">
         <v>2</v>
@@ -1871,7 +1874,7 @@
         <v>48</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>43</v>
@@ -1880,7 +1883,7 @@
         <v>54</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G13" s="5">
         <v>2</v>
@@ -1992,7 +1995,7 @@
         <v>54</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G14" s="5">
         <v>1</v>
@@ -2103,7 +2106,7 @@
         <v>54</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G15" s="5">
         <v>2</v>
@@ -2214,7 +2217,7 @@
         <v>54</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G16" s="5">
         <v>2</v>
@@ -2321,7 +2324,7 @@
         <v>49</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>43</v>
@@ -2330,7 +2333,7 @@
         <v>54</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G17" s="5">
         <v>2</v>
@@ -2442,7 +2445,7 @@
         <v>54</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G18" s="5">
         <v>1</v>
@@ -2554,7 +2557,7 @@
         <v>54</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G19" s="5">
         <v>2</v>
@@ -2666,7 +2669,7 @@
         <v>54</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G20" s="5">
         <v>2</v>
@@ -2773,7 +2776,7 @@
         <v>50</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>43</v>
@@ -2782,7 +2785,7 @@
         <v>54</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G21" s="5">
         <v>2</v>
@@ -2894,7 +2897,7 @@
         <v>54</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="G22" s="5">
         <v>1</v>
@@ -3004,7 +3007,7 @@
         <v>54</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="G23" s="5">
         <v>2</v>
@@ -3114,7 +3117,7 @@
         <v>54</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G24" s="5">
         <v>2</v>
@@ -3221,7 +3224,7 @@
         <v>51</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>43</v>
@@ -3230,7 +3233,7 @@
         <v>54</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G25" s="5">
         <v>2</v>
@@ -3342,7 +3345,7 @@
         <v>54</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G26" s="5">
         <v>1</v>
@@ -3454,7 +3457,7 @@
         <v>54</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G27" s="5">
         <v>2</v>
@@ -3566,7 +3569,7 @@
         <v>54</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G28" s="5">
         <v>2</v>
@@ -3673,7 +3676,7 @@
         <v>52</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>43</v>
@@ -3682,7 +3685,7 @@
         <v>54</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G29" s="5">
         <v>2</v>
@@ -3794,7 +3797,7 @@
         <v>54</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G30" s="5">
         <v>1</v>
@@ -3906,7 +3909,7 @@
         <v>54</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G31" s="5">
         <v>2</v>
@@ -4018,7 +4021,7 @@
         <v>54</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G32" s="5">
         <v>2</v>
@@ -4125,7 +4128,7 @@
         <v>53</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>43</v>
@@ -4134,7 +4137,7 @@
         <v>54</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G33" s="5">
         <v>2</v>
@@ -4246,7 +4249,7 @@
         <v>54</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G34" s="5">
         <v>1</v>
@@ -4358,7 +4361,7 @@
         <v>54</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G35" s="5">
         <v>2</v>
@@ -4470,7 +4473,7 @@
         <v>54</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G36" s="5">
         <v>2</v>
@@ -4574,10 +4577,10 @@
     </row>
     <row r="37" spans="2:53" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B37" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>43</v>
@@ -4586,7 +4589,7 @@
         <v>54</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G37" s="5">
         <v>2</v>
@@ -4698,7 +4701,7 @@
         <v>54</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G38" s="5">
         <v>1</v>
@@ -4810,7 +4813,7 @@
         <v>54</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G39" s="5">
         <v>2</v>
@@ -4922,7 +4925,7 @@
         <v>54</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G40" s="5">
         <v>2</v>
@@ -5026,10 +5029,10 @@
     </row>
     <row r="41" spans="2:53" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B41" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>43</v>
@@ -5038,7 +5041,7 @@
         <v>54</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G41" s="5">
         <v>2</v>
@@ -5150,7 +5153,7 @@
         <v>54</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="G42" s="5">
         <v>1</v>
@@ -5260,7 +5263,7 @@
         <v>54</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="G43" s="5">
         <v>2</v>
@@ -5370,7 +5373,7 @@
         <v>54</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G44" s="5">
         <v>2</v>
@@ -5474,10 +5477,10 @@
     </row>
     <row r="45" spans="2:53" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B45" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>43</v>
@@ -5486,7 +5489,7 @@
         <v>54</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G45" s="5">
         <v>2</v>
@@ -5598,7 +5601,7 @@
         <v>54</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G46" s="5">
         <v>1</v>
@@ -5710,7 +5713,7 @@
         <v>54</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G47" s="5">
         <v>2</v>
@@ -5822,7 +5825,7 @@
         <v>54</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G48" s="5">
         <v>2</v>
@@ -5926,10 +5929,10 @@
     </row>
     <row r="49" spans="2:53" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B49" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>43</v>
@@ -5938,7 +5941,7 @@
         <v>54</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G49" s="5">
         <v>2</v>
@@ -6050,7 +6053,7 @@
         <v>54</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G50" s="5">
         <v>2</v>
@@ -6162,7 +6165,7 @@
         <v>54</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G51" s="5">
         <v>2</v>
@@ -6274,7 +6277,7 @@
         <v>54</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="G52" s="5">
         <v>2</v>
@@ -6376,10 +6379,10 @@
     </row>
     <row r="53" spans="2:53" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B53" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D53" s="5" t="s">
         <v>43</v>
@@ -6388,7 +6391,7 @@
         <v>54</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G53" s="5">
         <v>2</v>
@@ -6500,7 +6503,7 @@
         <v>54</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G54" s="5">
         <v>2</v>
@@ -6612,7 +6615,7 @@
         <v>54</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G55" s="5">
         <v>2</v>
@@ -6724,7 +6727,7 @@
         <v>54</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G56" s="5">
         <v>2</v>
@@ -6828,6 +6831,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -6839,11 +6847,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -6912,7 +6915,7 @@
         <v>4</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
@@ -6963,7 +6966,7 @@
         <v>47</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>43</v>
@@ -7019,7 +7022,7 @@
         <v>48</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>43</v>
@@ -7075,7 +7078,7 @@
         <v>49</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>43</v>
@@ -7131,7 +7134,7 @@
         <v>50</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>43</v>
@@ -7183,7 +7186,7 @@
         <v>51</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>43</v>
@@ -7239,7 +7242,7 @@
         <v>52</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>43</v>
@@ -7295,7 +7298,7 @@
         <v>53</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>43</v>
@@ -7348,10 +7351,10 @@
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B36" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>43</v>
@@ -7404,10 +7407,10 @@
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B40" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>43</v>
@@ -7456,10 +7459,10 @@
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B44" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D44" s="5" t="s">
         <v>43</v>
@@ -7512,10 +7515,10 @@
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B48" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>43</v>
@@ -7566,10 +7569,10 @@
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B52" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D52" s="5" t="s">
         <v>43</v>

</xml_diff>